<commit_message>
Tag tasks, update spreadsheet w/total lbs
</commit_message>
<xml_diff>
--- a/Quantities-for-Soup.xlsx
+++ b/Quantities-for-Soup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\teleflex\global\Home\Medical\NA\MOR\Home2\elusk\Misc\ZOE\Soup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j6l\Documents\Zoe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF40725A-2F65-4FC7-A58D-21FD572EF600}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63186083-A00D-43D0-B106-ABAD28AF42F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{08AA109B-3210-4AF6-9B01-137F7C5D01DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{08AA109B-3210-4AF6-9B01-137F7C5D01DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="53">
   <si>
     <t>Bay Leaves</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Fabric Scraps (5"x5"?)</t>
+  </si>
+  <si>
+    <t>(total lbs)</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +598,7 @@
     <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -614,7 +617,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -625,7 +628,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -653,7 +656,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -683,7 +686,7 @@
         <v>Rolls</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -713,7 +716,7 @@
         <v>Rolls</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -742,7 +745,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -772,7 +775,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -801,7 +804,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -831,7 +834,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -861,7 +864,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -890,7 +893,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -919,7 +922,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -948,7 +951,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -977,7 +980,7 @@
         <v>lb</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1005,6 +1008,13 @@
         <f t="shared" si="3"/>
         <v>lb</v>
       </c>
+      <c r="L16" s="6">
+        <f>SUM(J7:J16,J18)</f>
+        <v>1252</v>
+      </c>
+      <c r="M16" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1150,7 +1160,7 @@
         <v>18</v>
       </c>
       <c r="J22" s="6">
-        <f>ROUNDUP(D13+D31,0)</f>
+        <f t="shared" ref="J22:J27" si="9">ROUNDUP(D13+D31,0)</f>
         <v>2600</v>
       </c>
       <c r="K22" t="s">
@@ -1169,7 +1179,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="6">
-        <f t="shared" ref="D23" si="9">B23*$D$1</f>
+        <f t="shared" ref="D23" si="10">B23*$D$1</f>
         <v>36.111111111111107</v>
       </c>
       <c r="E23" t="s">
@@ -1179,7 +1189,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="6">
-        <f>ROUNDUP(D14+D32,0)</f>
+        <f t="shared" si="9"/>
         <v>1300</v>
       </c>
       <c r="K23" t="s">
@@ -1197,7 +1207,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="6">
-        <f>B24*$G$1</f>
+        <f t="shared" ref="D24:D36" si="11">B24*$G$1</f>
         <v>95.333333333333329</v>
       </c>
       <c r="E24" t="s">
@@ -1207,7 +1217,7 @@
         <v>7</v>
       </c>
       <c r="J24" s="6">
-        <f>ROUNDUP(D15+D33,0)</f>
+        <f t="shared" si="9"/>
         <v>1300</v>
       </c>
       <c r="K24" t="s">
@@ -1225,7 +1235,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="6">
-        <f>B25*$G$1</f>
+        <f t="shared" si="11"/>
         <v>95.333333333333329</v>
       </c>
       <c r="E25" t="s">
@@ -1235,7 +1245,7 @@
         <v>10</v>
       </c>
       <c r="J25" s="6">
-        <f>ROUNDUP(D16+D34,0)</f>
+        <f t="shared" si="9"/>
         <v>1300</v>
       </c>
       <c r="K25" t="s">
@@ -1253,7 +1263,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="6">
-        <f>B26*$G$1</f>
+        <f t="shared" si="11"/>
         <v>95.333333333333329</v>
       </c>
       <c r="E26" t="s">
@@ -1263,7 +1273,7 @@
         <v>11</v>
       </c>
       <c r="J26" s="6">
-        <f>ROUNDUP(D17+D35,0)</f>
+        <f t="shared" si="9"/>
         <v>1300</v>
       </c>
       <c r="K26" t="s">
@@ -1281,7 +1291,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="6">
-        <f>B27*$G$1</f>
+        <f t="shared" si="11"/>
         <v>95.333333333333329</v>
       </c>
       <c r="E27" t="s">
@@ -1291,7 +1301,7 @@
         <v>11</v>
       </c>
       <c r="J27" s="6">
-        <f>ROUNDUP(D18+D36,0)</f>
+        <f t="shared" si="9"/>
         <v>1300</v>
       </c>
       <c r="K27" t="s">
@@ -1310,7 +1320,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="6">
-        <f>B28*$G$1</f>
+        <f t="shared" si="11"/>
         <v>95.333333333333329</v>
       </c>
       <c r="E28" t="s">
@@ -1338,7 +1348,7 @@
         <v>17</v>
       </c>
       <c r="D29" s="6">
-        <f>B29*$G$1</f>
+        <f t="shared" si="11"/>
         <v>95.333333333333329</v>
       </c>
       <c r="E29" t="s">
@@ -1360,7 +1370,7 @@
         <v>17</v>
       </c>
       <c r="D30" s="6">
-        <f>B30*$G$1</f>
+        <f t="shared" si="11"/>
         <v>95.333333333333329</v>
       </c>
       <c r="E30" t="s">
@@ -1378,7 +1388,7 @@
         <v>15</v>
       </c>
       <c r="D31" s="6">
-        <f>B31*$G$1</f>
+        <f t="shared" si="11"/>
         <v>1300</v>
       </c>
       <c r="E31" t="s">
@@ -1396,7 +1406,7 @@
         <v>15</v>
       </c>
       <c r="D32" s="6">
-        <f>B32*$G$1</f>
+        <f t="shared" si="11"/>
         <v>650</v>
       </c>
       <c r="E32" t="s">
@@ -1414,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="D33" s="6">
-        <f>B33*$G$1</f>
+        <f t="shared" si="11"/>
         <v>650</v>
       </c>
       <c r="E33" t="s">
@@ -1432,7 +1442,7 @@
         <v>15</v>
       </c>
       <c r="D34" s="6">
-        <f>B34*$G$1</f>
+        <f t="shared" si="11"/>
         <v>650</v>
       </c>
       <c r="E34" t="s">
@@ -1450,7 +1460,7 @@
         <v>15</v>
       </c>
       <c r="D35" s="6">
-        <f>B35*$G$1</f>
+        <f t="shared" si="11"/>
         <v>650</v>
       </c>
       <c r="E35" t="s">
@@ -1475,7 +1485,7 @@
         <v>15</v>
       </c>
       <c r="D36" s="6">
-        <f>B36*$G$1</f>
+        <f t="shared" si="11"/>
         <v>650</v>
       </c>
       <c r="E36" t="s">

</xml_diff>